<commit_message>
add extra immune marker
</commit_message>
<xml_diff>
--- a/src/ScTypeDB_Immune_added.xlsx
+++ b/src/ScTypeDB_Immune_added.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WeChat\WeChat Files\lx563624348\FileStorage\File\2023-07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\1Research\IgA_Tianyi\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37444903-0491-4B68-A0A0-1ACC83A39F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84A94D6-2FC6-4E94-A688-42D31ECB96C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="312">
   <si>
     <t>tissueType</t>
   </si>
@@ -801,9 +802,6 @@
     <t>CD4,CD2,CD3D,CD3E,CD3G,CD3Z,CD25,CD45RA,CD62L,CD27,CD127,FOXP3,CCR7,CD45,CCR6,CD11b,CD30,CD6,CTLA4,IL2RA,GZMB,PTPRC</t>
   </si>
   <si>
-    <t>IGHG1, MZB1, SDC1, CD79A</t>
-  </si>
-  <si>
     <t>Plasma cells</t>
   </si>
   <si>
@@ -816,172 +814,74 @@
     <t>Activated CD4 T cell</t>
   </si>
   <si>
-    <t xml:space="preserve">AIM2 BIRC3 BRIP1 CCL20 CCL4 CCL5 CCNB1 CCR7 DUSP2 ESCO2 ETS1 EXO1 EXOC6 IARS ITK KIF11 KNTC1 NUF2 PRC1 PSAT1 RGS1 RTKN2 SAMSN1 SELL TRAT1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADRM1 AHSA1 C1GALT1C1 CCT6B CD37 CD3D CD3E CD3G CD69 CD8A CETN3 CSE1L GEMIN6 GNLY GPT2 GZMA GZMH GZMK IL2RB LCK MPZL1 NKG7 PIK3IP1 PTRH2 TIMM13 ZAP70 </t>
-  </si>
-  <si>
     <t>Central memory CD4 T cell</t>
   </si>
   <si>
-    <t xml:space="preserve">ABHD3 AHNAK ANXA2P2 AQP3 ATHL1 BMI1 BZW2 CD63 COL4A1 CYLD ELMO2 FYN GLIPR1 GSS IFITM2 ITGB1 ITGB2 KLF5 LSP1 NDUFB9 PKM2 SFXN3 SIRPG SMAD4 STX4 TRADD VIM XRCC6 </t>
-  </si>
-  <si>
     <t>Central memory CD8 T cell</t>
   </si>
   <si>
-    <t xml:space="preserve">ACTN4 ADAM12 ADCY9 F13A1 FCER1G FCGR3B FGF7 FKBP4 GLUD1 GM2A GUSB IL1RN NOL11 NTRK1 RARA RNF128 SIGLEC1 TNFRSF11A TOX4 UBA52 ULBP1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATM CASP3 CASQ1 CD300E DARS DOCK9 EXOSC9 EZH2 GDE1 IL34 NCOA4 NEFL PDGFRL PTGS1 REPS1 SCG2 SDPR SIGLEC14 SIGLEC6 TAL1 TFEC TIPIN TPK1 UQCRB USP9Y WIPF1 ZCRB1 </t>
-  </si>
-  <si>
     <t>Effector memeory CD8 T cell</t>
   </si>
   <si>
     <t>Gamma delta T cell</t>
   </si>
   <si>
-    <t xml:space="preserve">ACP5 AQP9 BTN3A2 C1orf54 CARD8 CCL18 CD209 CD33 CD36 CDK5 IL10RB KLRF1 LGALS1 MAPK7 KLHL7 KRT80 LAMC1 LCORL LMNB1 MEIS3P1 MPL FABP1 FABP5 FADD MFAP3L MINPP1 RPS24 RPS7 RPS9 DBNL CCL13 </t>
-  </si>
-  <si>
     <t>Regulatory T cell</t>
   </si>
   <si>
-    <t xml:space="preserve">CCL3L1 CD72 CLEC5A FOXP3 ITGA4 L1CAM LIPA LRP1 LRRC42 MARCO MMP12 MNDA MRC1 MS4A6A PELO PLEK PRSS23 PTGIR ST8SIA4 STAB1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">B3GAT1 CDK5R1 PDCD1 BCL6 CD200 CD83 CD84 FGF2 GPR18 CEBPA CECR1 CLEC10A CLEC4A CSF1R CTSS DMN DPP4 LRRC32 MC5R MICA NCAM1 NCR2 NRP1 PDCD1LG2 PDCD6 PRDX1 RAE1 RAET1E SIGLEC7 SIGLEC9 TYRO3 CHST12 CLIC3 IVNS1ABP KIR2DL2 LGMN </t>
-  </si>
-  <si>
     <t>T follicular helper cell</t>
   </si>
   <si>
     <t>Type 1 T helper cell</t>
   </si>
   <si>
-    <t xml:space="preserve">CD70 TBX21 ADAM8 AHCYL2 ALCAM B3GALNT1 BBS12 BST1 CD151 CD47 CD48 CD52 CD53 CD59 CD6 CD68 CD7 CD96 CFHR3 CHRM3 CLEC7A COL23A1 COL4A4 COL5A3 DAB1 DLEU7 DOC2B EMP1 F12 FURIN GAB3 GATM GFPT2 GPR25 GREM2 HAVCR1 HSD11B1 HUNK IGF2 RCSD1 RYR1 SAV1 SELE SELP SH3KBP1 SIT1 SLC35B3 SIGLEC10 SKAP1 THUMPD2 TIGIT ZEB2 ENC1 FAM134B FBXO30 FCGR2C STAC LTC4S MAN1B1 MDH1 MMD RGS16 IL12A P2RX5 CD97 ITGB4 ICAM3 METRNL TNFRSF1A IRF1 HTR2B CALD1 MOCOS TRAF3IP2 TLR8 TRAF1 DUSP14 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL17A IL17RA C2CD4A C2CD4B CA2 CCDC65 CEACAM3 IL17C IL17F IL17RC IL17RE IL23A ILDR1 LONRF3 SH2D6 TNIP2 ABCA1 ABCB1 ADAMTS12 ANK1 ANKRD22 B3GALT2 CAMTA1 CCR9 CD40 GPR44 IFT80 </t>
-  </si>
-  <si>
     <t>Type 17 T helper cell</t>
   </si>
   <si>
-    <t xml:space="preserve">ASB2 CSRP2 DAPK1 DLC1 DNAJC12 DUSP6 GNAI1 LAMP3 NRP2 OSBPL1A PDE4B PHLDA1 PLA2G4A RAB27B RBMS3 RNF125 TMPRSS3 GATA3 BIRC5 CDC25C CDC7 CENPF CXCR6 DHFR EVI5 GSTA4 HELLS IL26 LAIR2 </t>
-  </si>
-  <si>
     <t>Type 2 T helper cell</t>
   </si>
   <si>
     <t>Activated dendritic cell</t>
   </si>
   <si>
-    <t xml:space="preserve">ABCD1 C1QC CAPG CCL3L3 CD207 CD302 ATP5B ATP5L ATP6V1A BCL2L1 C1QB SNURF SPCS3 CCNA1 CEACAM8 NOS2 SRA1 TNFRSF6B TREM1 TREML1 RHOA SLC25A37 TNFSF14 TREML4 VNN2 XPO6 CLEC4C TNFAIP2 UBD ACTR3 RAB1A SLA HLA-DQA2 SIGLEC5 SLAMF9 </t>
-  </si>
-  <si>
     <t>CD56bright natural killer cell</t>
   </si>
   <si>
-    <t xml:space="preserve">ABAT C11orf75 C5orf15 CDHR1 DCAF12 DYNLL1 GPR137B HCP5 HDGFRP2 KRT86 MLST8 ELMOD3 ENTPD5 FAM119A FAM179A CLIC2 COX7A2L CREB3L4 CSF1 CSNK2A2 CSTA CSTB CTPS CTSD FST GATA2 GMPR HDC HEY1 HOXA1 HS2ST1 HS3ST1 BCL11B CDH3 MYL6B NAA16 ClQA ClQB CYP27B1 EIF3M </t>
-  </si>
-  <si>
     <t>CD56dim natural killer cell</t>
   </si>
   <si>
-    <t xml:space="preserve">CYP27A1 DDX55 DYRK2 RPL37A NOTCH3 AKR7A3 GPRC5C GRIN1 HLA-E PORCN PSMC4 UPP1 IL21R KIR2DS1 KIR2DS2 KIR2DS5 </t>
-  </si>
-  <si>
     <t>Immature dendritic cell</t>
   </si>
   <si>
-    <t xml:space="preserve">ACADM AHCYL1 ALDH1A2 ALDH3A2 ALDH9A1 ALOX15 AMT ARL1 ATIC ATP5A1 CAPZA1 LILRA5 RDX RRAGD TACSTD2 INPP5F RAB38 PLAU CSF3R SLC18A2 AMPD2 CLTB C1orf162 </t>
-  </si>
-  <si>
     <t>MDSC</t>
   </si>
   <si>
-    <t xml:space="preserve">CCR2 CD14 CD2 CD86 CXCR4 FCGR2A FCGR2B FCGR3A FERMT3 GPSM3 IL18BP IL4R ITGAL ITGAM PARVG PSAP PTGER2 PTGES2 S100A8 S100A9 </t>
-  </si>
-  <si>
     <t>Monocyte</t>
   </si>
   <si>
-    <t xml:space="preserve">ASGR2 CFP ASGR1 CD1D UPK3A ACTG1 ANXA5 ATP6V1B2 CFL1 DAZAP2 CTBS EMR4P HIVEP2 MARCKSL1 MBP MMP15 PNPLA6 TMBIM6 PQBP1 TEX264 IKZF1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CBX6 DAB2 DDX17 HIGD1A IDH3A IL3RA MAGED1 NUCB2 OFD1 OGT PDIA4 SERTAD2 SIRPA TMED2 ENG FCAR IGF1 ITGA2B GABARAP GPX1 KRT23 PROK2 RALB RETNLB RNF141 SEC14L1 SEPX1 EMP3 CD300LF ABTB1 KLHL21 PHRF1 </t>
-  </si>
-  <si>
     <t>Plasmacytoid dendritic cell</t>
-  </si>
-  <si>
-    <r>
-      <t>ADAM28</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CD180 CD79B BLK CD19 MS4A1 TNFRSF17 IGHM GNG7 MICAL3 SPIB HLA-DOB IGKC PNOC FCRL2 BACH2 CR2 TCL1A AKNA ARHGAP25 CCL21 CD27 CD38 CLEC17A CLEC9A CLECL1 </t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Central memory CD8 T cell</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">GPR183 CCR7 SELL IL7R CD27 CD28 GZMA CCL5 S1PR1 GZMA CCL5 S1PR1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CX3CR1 KLRG1 FCGR3A FGFBP2 PRF1 GZMH TBX21 EOMES S1PR1 S1PR5 </t>
-  </si>
-  <si>
     <t>Temra CD8 T cell</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">LAYN CXCL13 HAVCR2 PDCD1 TOX IFNG GZMB MIR155HG TNFRSF9 ITGAE </t>
-  </si>
-  <si>
     <t>exhausted CD8 T cell</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">NKG7 CCL4 CST7 GZMA  GZMB IFNG CCL3 </t>
-  </si>
-  <si>
     <t>cytotoxic CD8 T cell</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">CD6 CXCL1 XCL2 MYADM CAPG RORA NR4A1 NR4A2 NR4A3 CD69 ITGAE </t>
-  </si>
-  <si>
     <t>Tissue Resident Memory T cell (Trm)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>CCL18 CD206 CD14 HLA-DR ARG1 CCL2 CD163 MRC1 RETNLB IL10 MRC1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>M1 macrophage</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -990,15 +890,92 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>FCGR3A TSPO CD68 HLA-DR CXCL10 ROS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>ADAM28,CD180,CD79B,BLK,CD19,MS4A1,TNFRSF17,IGHM,GNG7,MICAL3,SPIB,HLA-DOB,IGKC,PNOC,FCRL2,BACH2,CR2,TCL1A,AKNA,ARHGAP25,CCL21,CD27,CD38,CLEC17A,CLEC9A,CLECL1,</t>
+  </si>
+  <si>
+    <t>AIM2,BIRC3,BRIP1,CCL20,CCL4,CCL5,CCNB1,CCR7,DUSP2,ESCO2,ETS1,EXO1,EXOC6,IARS,ITK,KIF11,KNTC1,NUF2,PRC1,PSAT1,RGS1,RTKN2,SAMSN1,SELL,TRAT1,</t>
+  </si>
+  <si>
+    <t>ADRM1,AHSA1,C1GALT1C1,CCT6B,CD37,CD3D,CD3E,CD3G,CD69,CD8A,CETN3,CSE1L,GEMIN6,GNLY,GPT2,GZMA,GZMH,GZMK,IL2RB,LCK,MPZL1,NKG7,PIK3IP1,PTRH2,TIMM13,ZAP70,</t>
+  </si>
+  <si>
+    <t>ABHD3,AHNAK,ANXA2P2,AQP3,ATHL1,BMI1,BZW2,CD63,COL4A1,CYLD,ELMO2,FYN,GLIPR1,GSS,IFITM2,ITGB1,ITGB2,KLF5,LSP1,NDUFB9,PKM2,SFXN3,SIRPG,SMAD4,STX4,TRADD,VIM,XRCC6,</t>
+  </si>
+  <si>
+    <t>ACTN4,ADAM12,ADCY9,F13A1,FCER1G,FCGR3B,FGF7,FKBP4,GLUD1,GM2A,GUSB,IL1RN,NOL11,NTRK1,RARA,RNF128,SIGLEC1,TNFRSF11A,TOX4,UBA52,ULBP1,</t>
+  </si>
+  <si>
+    <t>ATM,CASP3,CASQ1,CD300E,DARS,DOCK9,EXOSC9,EZH2,GDE1,IL34,NCOA4,NEFL,PDGFRL,PTGS1,REPS1,SCG2,SDPR,SIGLEC14,SIGLEC6,TAL1,TFEC,TIPIN,TPK1,UQCRB,USP9Y,WIPF1,ZCRB1,</t>
+  </si>
+  <si>
+    <t>ACP5,AQP9,BTN3A2,C1orf54,CARD8,CCL18,CD209,CD33,CD36,CDK5,IL10RB,KLRF1,LGALS1,MAPK7,KLHL7,KRT80,LAMC1,LCORL,LMNB1,MEIS3P1,MPL,FABP1,FABP5,FADD,MFAP3L,MINPP1,RPS24,RPS7,RPS9,DBNL,CCL13,</t>
+  </si>
+  <si>
+    <t>CCL3L1,CD72,CLEC5A,FOXP3,ITGA4,L1CAM,LIPA,LRP1,LRRC42,MARCO,MMP12,MNDA,MRC1,MS4A6A,PELO,PLEK,PRSS23,PTGIR,ST8SIA4,STAB1,</t>
+  </si>
+  <si>
+    <t>B3GAT1,CDK5R1,PDCD1,BCL6,CD200,CD83,CD84,FGF2,GPR18,CEBPA,CECR1,CLEC10A,CLEC4A,CSF1R,CTSS,DMN,DPP4,LRRC32,MC5R,MICA,NCAM1,NCR2,NRP1,PDCD1LG2,PDCD6,PRDX1,RAE1,RAET1E,SIGLEC7,SIGLEC9,TYRO3,CHST12,CLIC3,IVNS1ABP,KIR2DL2,LGMN,</t>
+  </si>
+  <si>
+    <t>CD70,TBX21,ADAM8,AHCYL2,ALCAM,B3GALNT1,BBS12,BST1,CD151,CD47,CD48,CD52,CD53,CD59,CD6,CD68,CD7,CD96,CFHR3,CHRM3,CLEC7A,COL23A1,COL4A4,COL5A3,DAB1,DLEU7,DOC2B,EMP1,F12,FURIN,GAB3,GATM,GFPT2,GPR25,GREM2,HAVCR1,HSD11B1,HUNK,IGF2,RCSD1,RYR1,SAV1,SELE,SELP,SH3KBP1,SIT1,SLC35B3,SIGLEC10,SKAP1,THUMPD2,TIGIT,ZEB2,ENC1,FAM134B,FBXO30,FCGR2C,STAC,LTC4S,MAN1B1,MDH1,MMD,RGS16,IL12A,P2RX5,CD97,ITGB4,ICAM3,METRNL,TNFRSF1A,IRF1,HTR2B,CALD1,MOCOS,TRAF3IP2,TLR8,TRAF1,DUSP14,</t>
+  </si>
+  <si>
+    <t>IL17A,IL17RA,C2CD4A,C2CD4B,CA2,CCDC65,CEACAM3,IL17C,IL17F,IL17RC,IL17RE,IL23A,ILDR1,LONRF3,SH2D6,TNIP2,ABCA1,ABCB1,ADAMTS12,ANK1,ANKRD22,B3GALT2,CAMTA1,CCR9,CD40,GPR44,IFT80,</t>
+  </si>
+  <si>
+    <t>ASB2,CSRP2,DAPK1,DLC1,DNAJC12,DUSP6,GNAI1,LAMP3,NRP2,OSBPL1A,PDE4B,PHLDA1,PLA2G4A,RAB27B,RBMS3,RNF125,TMPRSS3,GATA3,BIRC5,CDC25C,CDC7,CENPF,CXCR6,DHFR,EVI5,GSTA4,HELLS,IL26,LAIR2,</t>
+  </si>
+  <si>
+    <t>ABCD1,C1QC,CAPG,CCL3L3,CD207,CD302,ATP5B,ATP5L,ATP6V1A,BCL2L1,C1QB,SNURF,SPCS3,CCNA1,CEACAM8,NOS2,SRA1,TNFRSF6B,TREM1,TREML1,RHOA,SLC25A37,TNFSF14,TREML4,VNN2,XPO6,CLEC4C,TNFAIP2,UBD,ACTR3,RAB1A,SLA,HLA-DQA2,SIGLEC5,SLAMF9,</t>
+  </si>
+  <si>
+    <t>ABAT,C11orf75,C5orf15,CDHR1,DCAF12,DYNLL1,GPR137B,HCP5,HDGFRP2,KRT86,MLST8,ELMOD3,ENTPD5,FAM119A,FAM179A,CLIC2,COX7A2L,CREB3L4,CSF1,CSNK2A2,CSTA,CSTB,CTPS,CTSD,FST,GATA2,GMPR,HDC,HEY1,HOXA1,HS2ST1,HS3ST1,BCL11B,CDH3,MYL6B,NAA16,ClQA,ClQB,CYP27B1,EIF3M,</t>
+  </si>
+  <si>
+    <t>CYP27A1,DDX55,DYRK2,RPL37A,NOTCH3,AKR7A3,GPRC5C,GRIN1,HLA-E,PORCN,PSMC4,UPP1,IL21R,KIR2DS1,KIR2DS2,KIR2DS5,</t>
+  </si>
+  <si>
+    <t>ACADM,AHCYL1,ALDH1A2,ALDH3A2,ALDH9A1,ALOX15,AMT,ARL1,ATIC,ATP5A1,CAPZA1,LILRA5,RDX,RRAGD,TACSTD2,INPP5F,RAB38,PLAU,CSF3R,SLC18A2,AMPD2,CLTB,C1orf162,</t>
+  </si>
+  <si>
+    <t>CCR2,CD14,CD2,CD86,CXCR4,FCGR2A,FCGR2B,FCGR3A,FERMT3,GPSM3,IL18BP,IL4R,ITGAL,ITGAM,PARVG,PSAP,PTGER2,PTGES2,S100A8,S100A9,</t>
+  </si>
+  <si>
+    <t>ASGR2,CFP,ASGR1,CD1D,UPK3A,ACTG1,ANXA5,ATP6V1B2,CFL1,DAZAP2,CTBS,EMR4P,HIVEP2,MARCKSL1,MBP,MMP15,PNPLA6,TMBIM6,PQBP1,TEX264,IKZF1,</t>
+  </si>
+  <si>
+    <t>CBX6,DAB2,DDX17,HIGD1A,IDH3A,IL3RA,MAGED1,NUCB2,OFD1,OGT,PDIA4,SERTAD2,SIRPA,TMED2,ENG,FCAR,IGF1,ITGA2B,GABARAP,GPX1,KRT23,PROK2,RALB,RETNLB,RNF141,SEC14L1,SEPX1,EMP3,CD300LF,ABTB1,KLHL21,PHRF1,</t>
+  </si>
+  <si>
+    <t>GPR183,CCR7,SELL,IL7R,CD27,CD28,GZMA,CCL5,S1PR1,GZMA,CCL5,S1PR1,</t>
+  </si>
+  <si>
+    <t>CX3CR1,KLRG1,FCGR3A,FGFBP2,PRF1,GZMH,TBX21,EOMES,S1PR1,S1PR5,</t>
+  </si>
+  <si>
+    <t>LAYN,CXCL13,HAVCR2,PDCD1,TOX,IFNG,GZMB,MIR155HG,TNFRSF9,ITGAE,</t>
+  </si>
+  <si>
+    <t>NKG7,CCL4,CST7,GZMA,,GZMB,IFNG,CCL3,</t>
+  </si>
+  <si>
+    <t>CD6,CXCL1,XCL2,MYADM,CAPG,RORA,NR4A1,NR4A2,NR4A3,CD69,ITGAE,</t>
+  </si>
+  <si>
+    <t>FCGR3A,TSPO,CD68,HLA-DR,CXCL10,ROS</t>
+  </si>
+  <si>
+    <t>CCL18,CD206,CD14,HLA-DR,ARG1,CCL2,CD163,MRC1,RETNLB,IL10,MRC1</t>
+  </si>
+  <si>
+    <t>IGHG1,MZB1,SDC1,CD79A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1023,19 +1000,6 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1378,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127:XFD127"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3028,10 +2992,10 @@
         <v>97</v>
       </c>
       <c r="B128" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C128" t="s">
-        <v>258</v>
+        <v>311</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -3039,10 +3003,10 @@
         <v>97</v>
       </c>
       <c r="B129" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C129" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -3050,10 +3014,10 @@
         <v>97</v>
       </c>
       <c r="B130" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C130" t="s">
-        <v>263</v>
+        <v>286</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -3061,10 +3025,10 @@
         <v>97</v>
       </c>
       <c r="B131" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C131" t="s">
-        <v>264</v>
+        <v>287</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -3072,10 +3036,10 @@
         <v>97</v>
       </c>
       <c r="B132" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C132" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -3083,10 +3047,10 @@
         <v>97</v>
       </c>
       <c r="B133" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C133" t="s">
-        <v>268</v>
+        <v>289</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -3094,10 +3058,10 @@
         <v>97</v>
       </c>
       <c r="B134" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C134" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -3105,10 +3069,10 @@
         <v>97</v>
       </c>
       <c r="B135" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C135" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -3116,10 +3080,10 @@
         <v>97</v>
       </c>
       <c r="B136" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C136" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -3127,10 +3091,10 @@
         <v>97</v>
       </c>
       <c r="B137" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C137" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -3138,10 +3102,10 @@
         <v>97</v>
       </c>
       <c r="B138" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C138" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -3149,10 +3113,10 @@
         <v>97</v>
       </c>
       <c r="B139" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="C139" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -3160,10 +3124,10 @@
         <v>97</v>
       </c>
       <c r="B140" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="C140" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -3171,10 +3135,10 @@
         <v>97</v>
       </c>
       <c r="B141" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="C141" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -3182,10 +3146,10 @@
         <v>97</v>
       </c>
       <c r="B142" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="C142" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -3193,10 +3157,10 @@
         <v>97</v>
       </c>
       <c r="B143" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="C143" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -3204,10 +3168,10 @@
         <v>97</v>
       </c>
       <c r="B144" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="C144" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -3215,10 +3179,10 @@
         <v>97</v>
       </c>
       <c r="B145" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="C145" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -3226,10 +3190,10 @@
         <v>97</v>
       </c>
       <c r="B146" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="C146" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -3237,10 +3201,10 @@
         <v>97</v>
       </c>
       <c r="B147" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="C147" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -3248,10 +3212,10 @@
         <v>97</v>
       </c>
       <c r="B148" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="C148" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -3259,10 +3223,10 @@
         <v>97</v>
       </c>
       <c r="B149" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="C149" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -3270,10 +3234,10 @@
         <v>97</v>
       </c>
       <c r="B150" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="C150" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -3281,10 +3245,10 @@
         <v>97</v>
       </c>
       <c r="B151" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="C151" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -3292,10 +3256,10 @@
         <v>97</v>
       </c>
       <c r="B152" t="s">
-        <v>307</v>
+        <v>282</v>
       </c>
       <c r="C152" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -3303,10 +3267,10 @@
         <v>97</v>
       </c>
       <c r="B153" t="s">
+        <v>283</v>
+      </c>
+      <c r="C153" t="s">
         <v>309</v>
-      </c>
-      <c r="C153" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -3314,10 +3278,10 @@
         <v>97</v>
       </c>
       <c r="B154" t="s">
+        <v>284</v>
+      </c>
+      <c r="C154" t="s">
         <v>310</v>
-      </c>
-      <c r="C154" t="s">
-        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3325,4 +3289,157 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B6DF26-1892-450B-A22B-529B346D19EF}">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A1:A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="57.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>310</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>